<commit_message>
made powershell script return frame width and length
</commit_message>
<xml_diff>
--- a/animations/fragment-a-accelerate-and-stretch.xlsx
+++ b/animations/fragment-a-accelerate-and-stretch.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53713207-0743-8F48-A0F6-476288695DF9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4095953-079F-4262-89EC-DBCABEAB5922}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="50360" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="50355" windowHeight="28335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -176,70 +176,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill>
@@ -635,20 +572,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:HI46"/>
+  <dimension ref="A1:GR46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1"/>
+    <sheetView tabSelected="1" topLeftCell="EP20" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
+      <selection activeCell="GG33" sqref="GG33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="20" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="217" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="20" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="217" width="2.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:217" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:200" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1249,59 +1186,8 @@
       <c r="GR1">
         <v>2</v>
       </c>
-      <c r="GS1">
-        <v>3</v>
-      </c>
-      <c r="GT1">
-        <v>4</v>
-      </c>
-      <c r="GU1">
-        <v>5</v>
-      </c>
-      <c r="GV1">
-        <v>6</v>
-      </c>
-      <c r="GW1">
-        <v>7</v>
-      </c>
-      <c r="GX1">
-        <v>8</v>
-      </c>
-      <c r="GY1">
-        <v>9</v>
-      </c>
-      <c r="GZ1">
-        <v>0</v>
-      </c>
-      <c r="HA1">
-        <v>1</v>
-      </c>
-      <c r="HB1">
-        <v>2</v>
-      </c>
-      <c r="HC1">
-        <v>3</v>
-      </c>
-      <c r="HD1">
-        <v>4</v>
-      </c>
-      <c r="HE1">
-        <v>5</v>
-      </c>
-      <c r="HF1">
-        <v>6</v>
-      </c>
-      <c r="HG1">
-        <v>7</v>
-      </c>
-      <c r="HH1">
-        <v>8</v>
-      </c>
-      <c r="HI1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:217" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:200" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1330,7 +1216,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:217" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:200" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -1359,7 +1245,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:217" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:200" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1</v>
       </c>
@@ -1390,7 +1276,7 @@
       <c r="T4" s="1"/>
       <c r="U4"/>
     </row>
-    <row r="5" spans="1:217" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:200" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>1</v>
       </c>
@@ -1421,7 +1307,7 @@
       <c r="S5" s="1"/>
       <c r="U5"/>
     </row>
-    <row r="6" spans="1:217" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:200" x14ac:dyDescent="0.25">
       <c r="F6">
         <v>1</v>
       </c>
@@ -1452,7 +1338,7 @@
       <c r="T6" s="1"/>
       <c r="U6"/>
     </row>
-    <row r="7" spans="1:217" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:200" x14ac:dyDescent="0.25">
       <c r="H7">
         <v>1</v>
       </c>
@@ -1481,7 +1367,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:217" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:200" x14ac:dyDescent="0.25">
       <c r="J8">
         <v>1</v>
       </c>
@@ -1512,7 +1398,7 @@
       <c r="U8"/>
       <c r="X8" s="1"/>
     </row>
-    <row r="9" spans="1:217" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:200" x14ac:dyDescent="0.25">
       <c r="L9" s="2">
         <v>1</v>
       </c>
@@ -1559,7 +1445,7 @@
       <c r="AK9" s="3"/>
       <c r="AL9" s="3"/>
     </row>
-    <row r="10" spans="1:217" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:200" x14ac:dyDescent="0.25">
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
@@ -1606,7 +1492,7 @@
       <c r="AK10" s="3"/>
       <c r="AL10" s="3"/>
     </row>
-    <row r="11" spans="1:217" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:200" x14ac:dyDescent="0.25">
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -1653,7 +1539,7 @@
       <c r="AK11" s="3"/>
       <c r="AL11" s="3"/>
     </row>
-    <row r="12" spans="1:217" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:200" x14ac:dyDescent="0.25">
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
@@ -1700,7 +1586,7 @@
       <c r="AK12" s="3"/>
       <c r="AL12" s="3"/>
     </row>
-    <row r="13" spans="1:217" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:200" x14ac:dyDescent="0.25">
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
@@ -1747,7 +1633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:217" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:200" x14ac:dyDescent="0.25">
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -1792,7 +1678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:217" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:200" x14ac:dyDescent="0.25">
       <c r="U15"/>
       <c r="AF15">
         <v>1</v>
@@ -1822,7 +1708,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:217" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:200" x14ac:dyDescent="0.25">
       <c r="U16"/>
       <c r="AJ16">
         <v>1</v>
@@ -1852,7 +1738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="17" spans="20:152" x14ac:dyDescent="0.25">
       <c r="U17"/>
       <c r="AN17" s="11">
         <v>1</v>
@@ -1889,7 +1775,7 @@
       </c>
       <c r="BF17" s="1"/>
     </row>
-    <row r="18" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="18" spans="20:152" x14ac:dyDescent="0.25">
       <c r="U18"/>
       <c r="AC18" s="1"/>
       <c r="AR18" s="11">
@@ -1927,7 +1813,7 @@
       </c>
       <c r="BL18" s="1"/>
     </row>
-    <row r="19" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="19" spans="20:152" x14ac:dyDescent="0.25">
       <c r="U19"/>
       <c r="Y19" s="1"/>
       <c r="AV19" s="11">
@@ -1965,7 +1851,7 @@
       </c>
       <c r="BR19" s="1"/>
     </row>
-    <row r="20" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="20" spans="20:152" x14ac:dyDescent="0.25">
       <c r="U20"/>
       <c r="W20" s="1"/>
       <c r="AZ20" s="11"/>
@@ -2005,7 +1891,7 @@
       </c>
       <c r="BX20" s="1"/>
     </row>
-    <row r="21" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="21" spans="20:152" x14ac:dyDescent="0.25">
       <c r="U21"/>
       <c r="X21" s="1"/>
       <c r="BF21" s="11">
@@ -2044,7 +1930,7 @@
       </c>
       <c r="CE21" s="1"/>
     </row>
-    <row r="22" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="22" spans="20:152" x14ac:dyDescent="0.25">
       <c r="T22" s="1"/>
       <c r="U22"/>
       <c r="BK22" s="11">
@@ -2083,7 +1969,7 @@
       </c>
       <c r="CL22" s="1"/>
     </row>
-    <row r="23" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="23" spans="20:152" x14ac:dyDescent="0.25">
       <c r="BP23" s="11">
         <v>1</v>
       </c>
@@ -2121,7 +2007,7 @@
       </c>
       <c r="CS23" s="1"/>
     </row>
-    <row r="24" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="24" spans="20:152" x14ac:dyDescent="0.25">
       <c r="BU24" s="11">
         <v>1</v>
       </c>
@@ -2158,7 +2044,7 @@
       </c>
       <c r="CZ24" s="1"/>
     </row>
-    <row r="25" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="25" spans="20:152" x14ac:dyDescent="0.25">
       <c r="BZ25" s="11"/>
       <c r="CA25" s="11">
         <v>1</v>
@@ -2196,7 +2082,7 @@
       </c>
       <c r="DH25" s="1"/>
     </row>
-    <row r="26" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="26" spans="20:152" x14ac:dyDescent="0.25">
       <c r="CG26" s="11">
         <v>1</v>
       </c>
@@ -2234,7 +2120,7 @@
       </c>
       <c r="DP26" s="1"/>
     </row>
-    <row r="27" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="27" spans="20:152" x14ac:dyDescent="0.25">
       <c r="CM27" s="11">
         <v>1</v>
       </c>
@@ -2271,7 +2157,7 @@
       </c>
       <c r="DX27" s="1"/>
     </row>
-    <row r="28" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="28" spans="20:152" x14ac:dyDescent="0.25">
       <c r="CS28" s="11">
         <v>1</v>
       </c>
@@ -2307,7 +2193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="29" spans="20:152" x14ac:dyDescent="0.25">
       <c r="CY29" s="11">
         <v>1</v>
       </c>
@@ -2343,7 +2229,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="30" spans="20:152" x14ac:dyDescent="0.25">
       <c r="U30"/>
       <c r="DE30" s="11">
         <v>1</v>
@@ -2380,7 +2266,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="31" spans="20:152" x14ac:dyDescent="0.25">
       <c r="U31"/>
       <c r="DK31" s="11">
         <v>1</v>
@@ -2428,7 +2314,7 @@
       <c r="EP31" s="15"/>
       <c r="EQ31" s="15"/>
     </row>
-    <row r="32" spans="20:152" x14ac:dyDescent="0.2">
+    <row r="32" spans="20:152" x14ac:dyDescent="0.25">
       <c r="U32"/>
       <c r="DQ32" s="11"/>
       <c r="DR32" s="11">
@@ -2480,7 +2366,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="20:200" x14ac:dyDescent="0.2">
+    <row r="33" spans="20:200" x14ac:dyDescent="0.25">
       <c r="U33"/>
       <c r="DR33" s="3"/>
       <c r="DS33" s="3"/>
@@ -2540,7 +2426,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="20:200" x14ac:dyDescent="0.2">
+    <row r="34" spans="20:200" x14ac:dyDescent="0.25">
       <c r="U34"/>
       <c r="EF34" s="11">
         <v>1</v>
@@ -2591,7 +2477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="20:200" x14ac:dyDescent="0.2">
+    <row r="35" spans="20:200" x14ac:dyDescent="0.25">
       <c r="U35"/>
       <c r="EM35" s="11">
         <v>1</v>
@@ -2642,7 +2528,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="20:200" x14ac:dyDescent="0.2">
+    <row r="36" spans="20:200" x14ac:dyDescent="0.25">
       <c r="U36"/>
       <c r="BF36" s="1"/>
       <c r="ET36" s="11">
@@ -2694,7 +2580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="20:200" x14ac:dyDescent="0.2">
+    <row r="37" spans="20:200" x14ac:dyDescent="0.25">
       <c r="U37"/>
       <c r="AC37" s="1"/>
       <c r="BL37" s="1"/>
@@ -2747,7 +2633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="20:200" x14ac:dyDescent="0.2">
+    <row r="38" spans="20:200" x14ac:dyDescent="0.25">
       <c r="U38"/>
       <c r="Y38" s="1"/>
       <c r="BR38" s="1"/>
@@ -2800,34 +2686,34 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="20:200" x14ac:dyDescent="0.2">
+    <row r="39" spans="20:200" x14ac:dyDescent="0.25">
       <c r="U39"/>
       <c r="W39" s="1"/>
       <c r="BX39" s="1"/>
     </row>
-    <row r="40" spans="20:200" x14ac:dyDescent="0.2">
+    <row r="40" spans="20:200" x14ac:dyDescent="0.25">
       <c r="U40"/>
       <c r="X40" s="1"/>
       <c r="CE40" s="1"/>
     </row>
-    <row r="41" spans="20:200" x14ac:dyDescent="0.2">
+    <row r="41" spans="20:200" x14ac:dyDescent="0.25">
       <c r="T41" s="1"/>
       <c r="U41"/>
       <c r="CL41" s="1"/>
     </row>
-    <row r="42" spans="20:200" x14ac:dyDescent="0.2">
+    <row r="42" spans="20:200" x14ac:dyDescent="0.25">
       <c r="CS42" s="1"/>
     </row>
-    <row r="43" spans="20:200" x14ac:dyDescent="0.2">
+    <row r="43" spans="20:200" x14ac:dyDescent="0.25">
       <c r="CZ43" s="1"/>
     </row>
-    <row r="44" spans="20:200" x14ac:dyDescent="0.2">
+    <row r="44" spans="20:200" x14ac:dyDescent="0.25">
       <c r="DH44" s="1"/>
     </row>
-    <row r="45" spans="20:200" x14ac:dyDescent="0.2">
+    <row r="45" spans="20:200" x14ac:dyDescent="0.25">
       <c r="DP45" s="1"/>
     </row>
-    <row r="46" spans="20:200" x14ac:dyDescent="0.2">
+    <row r="46" spans="20:200" x14ac:dyDescent="0.25">
       <c r="DX46" s="1"/>
     </row>
   </sheetData>
@@ -2842,12 +2728,12 @@
         <color rgb="FFF5F0FF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="24" priority="31">
+    <cfRule type="containsBlanks" dxfId="15" priority="31">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM13">
-    <cfRule type="containsBlanks" dxfId="23" priority="29">
+    <cfRule type="containsBlanks" dxfId="14" priority="29">
       <formula>LEN(TRIM(AM13))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="30">
@@ -2862,7 +2748,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB14:AX16 AU16:AY16">
-    <cfRule type="containsBlanks" dxfId="19" priority="27">
+    <cfRule type="containsBlanks" dxfId="13" priority="27">
       <formula>LEN(TRIM(AB14))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="28">
@@ -2877,7 +2763,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD17">
-    <cfRule type="containsBlanks" dxfId="18" priority="25">
+    <cfRule type="containsBlanks" dxfId="12" priority="25">
       <formula>LEN(TRIM(BD17))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="26">
@@ -2892,7 +2778,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ17:BD17">
-    <cfRule type="containsBlanks" dxfId="17" priority="23">
+    <cfRule type="containsBlanks" dxfId="11" priority="23">
       <formula>LEN(TRIM(AZ17))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="24">
@@ -2907,7 +2793,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI18">
-    <cfRule type="containsBlanks" dxfId="16" priority="21">
+    <cfRule type="containsBlanks" dxfId="10" priority="21">
       <formula>LEN(TRIM(BI18))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="22">
@@ -2922,7 +2808,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE18:BI18">
-    <cfRule type="containsBlanks" dxfId="15" priority="19">
+    <cfRule type="containsBlanks" dxfId="9" priority="19">
       <formula>LEN(TRIM(BE18))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="20">
@@ -2949,17 +2835,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CM23:XFD23 A1:XFD22 A23:CF23 A24:XFD25 A26:DB26 DF26:XFD26 A27:DI27 DM27:XFD27 A28:DP28 DT28:XFD28 A29:DW29 EA29:XFD29 A30:ED30 EH30:XFD30 A31:DJ31 ER31:XFD31 EF31:EK31 A32:DP32 ES32 EV32:XFD32 A33:DQ33 FC33:XFD33 A34:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="11" priority="13">
+    <cfRule type="containsBlanks" dxfId="8" priority="13">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD31 A32:DP32 ES32 EV32:XFD32 A33:DQ33 FC33:XFD33 A34:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="10" priority="12">
+    <cfRule type="containsBlanks" dxfId="7" priority="12">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ET32">
-    <cfRule type="containsBlanks" dxfId="9" priority="10">
+    <cfRule type="containsBlanks" dxfId="6" priority="10">
       <formula>LEN(TRIM(ET32))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="11">
@@ -2986,17 +2872,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ET32">
-    <cfRule type="containsBlanks" dxfId="8" priority="8">
+    <cfRule type="containsBlanks" dxfId="5" priority="8">
       <formula>LEN(TRIM(ET32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ET32">
-    <cfRule type="containsBlanks" dxfId="7" priority="7">
+    <cfRule type="containsBlanks" dxfId="4" priority="7">
       <formula>LEN(TRIM(ET32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="6" priority="6">
+    <cfRule type="containsBlanks" dxfId="3" priority="6">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>